<commit_message>
good results for 3 sources whole catchment
</commit_message>
<xml_diff>
--- a/Whole_Catchment/data/morph_data_3s_mix-2025.xlsx
+++ b/Whole_Catchment/data/morph_data_3s_mix-2025.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -180,12 +180,6 @@
     <t>Mix</t>
   </si>
   <si>
-    <t>NS</t>
-  </si>
-  <si>
-    <t>WS</t>
-  </si>
-  <si>
     <t>353</t>
   </si>
   <si>
@@ -196,12 +190,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -259,17 +261,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -553,7 +556,7 @@
   <dimension ref="A1:AT61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4899,8 +4902,8 @@
       <c r="C52" s="6">
         <v>43.225065000000001</v>
       </c>
-      <c r="D52" s="6" t="s">
-        <v>53</v>
+      <c r="D52" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="E52" s="6">
         <v>0.69</v>
@@ -4994,8 +4997,8 @@
       <c r="C53" s="6">
         <v>43.224445000000003</v>
       </c>
-      <c r="D53" s="6" t="s">
-        <v>53</v>
+      <c r="D53" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="E53" s="6">
         <v>0.33</v>
@@ -5097,8 +5100,8 @@
       <c r="C54" s="6">
         <v>43.224632999999898</v>
       </c>
-      <c r="D54" s="6" t="s">
-        <v>53</v>
+      <c r="D54" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="E54" s="6">
         <v>0.42</v>
@@ -5200,8 +5203,8 @@
       <c r="C55" s="6">
         <v>43.224711999999897</v>
       </c>
-      <c r="D55" s="6" t="s">
-        <v>53</v>
+      <c r="D55" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="E55" s="6">
         <v>0.3</v>
@@ -5307,8 +5310,8 @@
       <c r="C56" s="6">
         <v>43.225448999999898</v>
       </c>
-      <c r="D56" s="6" t="s">
-        <v>53</v>
+      <c r="D56" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="E56" s="6">
         <v>0.43</v>
@@ -5410,8 +5413,8 @@
       <c r="C57" s="6">
         <v>43.223865000000004</v>
       </c>
-      <c r="D57" s="6" t="s">
-        <v>54</v>
+      <c r="D57" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="E57" s="6">
         <v>1.51</v>
@@ -5513,8 +5516,8 @@
       <c r="C58" s="6">
         <v>43.223379999999899</v>
       </c>
-      <c r="D58" s="6" t="s">
-        <v>54</v>
+      <c r="D58" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="E58" s="6">
         <v>1.5</v>
@@ -5610,8 +5613,8 @@
       <c r="C59" s="6">
         <v>43.223039999999898</v>
       </c>
-      <c r="D59" s="6" t="s">
-        <v>54</v>
+      <c r="D59" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="E59" s="6">
         <v>0.19</v>
@@ -5709,8 +5712,8 @@
       <c r="C60" s="6">
         <v>43.221727999999899</v>
       </c>
-      <c r="D60" s="6" t="s">
-        <v>54</v>
+      <c r="D60" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="E60" s="6">
         <v>1.1100000000000001</v>
@@ -5822,7 +5825,7 @@
         <v>50.22</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
@@ -5853,7 +5856,7 @@
       </c>
       <c r="S61" s="5"/>
       <c r="T61" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="U61" s="5"/>
       <c r="V61" s="5">

</xml_diff>